<commit_message>
add Ei approx atempt
</commit_message>
<xml_diff>
--- a/kk_manual/A,E aprox.xlsx
+++ b/kk_manual/A,E aprox.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\majer\Desktop\BC\BP\PyroPara_0.1\kk_manual\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5D3F01C-B00E-4EC4-9630-53A843F7EE4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DF99E4C-C496-427D-9516-6F3BD5D3A506}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13620" xr2:uid="{56D9331B-6D62-4AA3-8793-FCAA25F689CB}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>heating rate [K]</t>
   </si>
@@ -47,6 +47,36 @@
   </si>
   <si>
     <t>1/Tp</t>
+  </si>
+  <si>
+    <t>1/tp e3</t>
+  </si>
+  <si>
+    <t>717,68201</t>
+  </si>
+  <si>
+    <t>701,841989</t>
+  </si>
+  <si>
+    <t>669,305</t>
+  </si>
+  <si>
+    <t>497,115</t>
+  </si>
+  <si>
+    <t>489,727</t>
+  </si>
+  <si>
+    <t>488,36201</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  #not accurate</t>
+  </si>
+  <si>
+    <t>Ei</t>
+  </si>
+  <si>
+    <t>Ai</t>
   </si>
 </sst>
 </file>
@@ -63,15 +93,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -108,11 +144,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -122,6 +180,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -155,7 +219,17 @@
   <c:chart>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.12480336832895889"/>
+          <c:y val="2.5428331875182269E-2"/>
+          <c:w val="0.78252296587926506"/>
+          <c:h val="0.82775444736074655"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
@@ -258,6 +332,56 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.2561806649168854"/>
+                  <c:y val="1.84044181977252E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="cs-CZ"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>MDF_mockup!$E$13:$G$13</c:f>
@@ -265,13 +389,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>1.5170156055395343E-3</c:v>
+                  <c:v>1.5134386007570008E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.5410505033070943E-3</c:v>
+                  <c:v>1.5389279046440876E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.5740174050752208E-3</c:v>
+                  <c:v>1.589729078370464E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -283,13 +407,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>-9.0699975776975137</c:v>
+                  <c:v>-9.0747189906610259</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-9.5493845185521344</c:v>
+                  <c:v>-9.5521411599539885</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-10.605663049377531</c:v>
+                  <c:v>-10.585798243466272</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -329,6 +453,50 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="cs-CZ"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>MDF_mockup!$E$14:$G$14</c:f>
@@ -336,13 +504,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>1.3875957267601997E-3</c:v>
+                  <c:v>1.3933747621735705E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.3824489616087148E-3</c:v>
+                  <c:v>1.4248221332907455E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.3877132066958994E-3</c:v>
+                  <c:v>1.4940871501034657E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -354,13 +522,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>-9.2483424394997282</c:v>
+                  <c:v>-9.2400301704482981</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-9.7666001037604477</c:v>
+                  <c:v>-9.7062192019285796</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-10.857611030336001</c:v>
+                  <c:v>-10.709894628146456</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -387,7 +555,7 @@
         <c:axId val="379074496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="1.0000000000000002E-3"/>
+          <c:min val="1.1000000000000003E-3"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -501,7 +669,7 @@
         <c:axId val="379267504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="-8"/>
+          <c:max val="-7"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -633,10 +801,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.91093022747156616"/>
-          <c:y val="0.14062335958005248"/>
-          <c:w val="5.6795931758530184E-2"/>
-          <c:h val="0.23437664041994752"/>
+          <c:x val="0.78037467191601062"/>
+          <c:y val="0.11747521143190434"/>
+          <c:w val="0.19568482064741904"/>
+          <c:h val="0.16493219597550307"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="1"/>
@@ -1606,10 +1774,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C900792-E97C-4612-95E0-6A6DB801ACB9}">
-  <dimension ref="D5:G14"/>
+  <dimension ref="D5:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" topLeftCell="B3" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1619,7 +1787,7 @@
     <col min="6" max="7" width="9.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="4:8" x14ac:dyDescent="0.35">
       <c r="D5" s="2" t="s">
         <v>0</v>
       </c>
@@ -1633,138 +1801,228 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="4:8" x14ac:dyDescent="0.35">
       <c r="D6" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E6">
-        <v>497.11500000000001</v>
-      </c>
-      <c r="F6">
-        <v>489.72699999999998</v>
-      </c>
-      <c r="G6">
-        <v>488.36201</v>
+      <c r="E6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="7" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="4:8" x14ac:dyDescent="0.35">
       <c r="D7" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E7">
-        <v>659.18899999999996</v>
+        <v>660.74698999999998</v>
       </c>
       <c r="F7">
-        <v>648.90800000000002</v>
+        <v>649.80301999999995</v>
       </c>
       <c r="G7">
-        <v>635.31699000000003</v>
+        <v>629.03800000000001</v>
       </c>
     </row>
-    <row r="8" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="4:8" x14ac:dyDescent="0.35">
       <c r="D8" s="2"/>
-      <c r="E8" s="1">
-        <v>720.67100000000005</v>
-      </c>
-      <c r="F8" s="1">
-        <v>723.35401000000002</v>
-      </c>
-      <c r="G8" s="1">
-        <v>720.60999000000004</v>
+      <c r="E8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
-    <row r="9" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="4:8" x14ac:dyDescent="0.35">
       <c r="D9" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="8">
         <f>LN(($E$5/(E6^2)))</f>
         <v>-8.5056197698927694</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="8">
         <f>LN(($F$5/(F6^2)))</f>
         <v>-8.986498804309397</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="8">
         <f>LN(($G$5/(G6^2)))</f>
         <v>-10.079528816222727</v>
       </c>
+      <c r="H9" s="8">
+        <v>1</v>
+      </c>
     </row>
-    <row r="10" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="4:8" x14ac:dyDescent="0.35">
       <c r="D10" s="3"/>
       <c r="E10">
         <f t="shared" ref="E10:E11" si="0">LN(($E$5/(E7^2)))</f>
-        <v>-9.0699975776975137</v>
+        <v>-9.0747189906610259</v>
       </c>
       <c r="F10">
         <f t="shared" ref="F10:F11" si="1">LN(($F$5/(F7^2)))</f>
-        <v>-9.5493845185521344</v>
+        <v>-9.5521411599539885</v>
       </c>
       <c r="G10">
         <f t="shared" ref="G10:G11" si="2">LN(($G$5/(G7^2)))</f>
-        <v>-10.605663049377531</v>
+        <v>-10.585798243466272</v>
+      </c>
+      <c r="H10">
+        <v>2</v>
       </c>
     </row>
-    <row r="11" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="4:8" x14ac:dyDescent="0.35">
       <c r="D11" s="2"/>
-      <c r="E11">
-        <f t="shared" si="0"/>
-        <v>-9.2483424394997282</v>
-      </c>
-      <c r="F11">
+      <c r="E11" s="5">
+        <f>LN(($E$5/(E8^2)))</f>
+        <v>-9.2400301704482981</v>
+      </c>
+      <c r="F11" s="1">
         <f t="shared" si="1"/>
-        <v>-9.7666001037604477</v>
-      </c>
-      <c r="G11">
+        <v>-9.7062192019285796</v>
+      </c>
+      <c r="G11" s="1">
         <f t="shared" si="2"/>
-        <v>-10.857611030336001</v>
+        <v>-10.709894628146456</v>
+      </c>
+      <c r="H11">
+        <v>3</v>
       </c>
     </row>
-    <row r="12" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="4:8" x14ac:dyDescent="0.35">
       <c r="D12" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="8">
         <f>1/E6</f>
         <v>2.0116069722297659E-3</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="8">
         <f t="shared" ref="F12:G12" si="3">1/F6</f>
         <v>2.0419539866088658E-3</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="8">
         <f t="shared" si="3"/>
         <v>2.0476613240247741E-3</v>
       </c>
+      <c r="H12" s="8" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="13" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="4:8" x14ac:dyDescent="0.35">
       <c r="D13" s="4"/>
       <c r="E13">
         <f>1/E7</f>
-        <v>1.5170156055395343E-3</v>
+        <v>1.5134386007570008E-3</v>
       </c>
       <c r="F13">
-        <f t="shared" ref="E13:G13" si="4">1/F7</f>
-        <v>1.5410505033070943E-3</v>
+        <f t="shared" ref="F13:G13" si="4">1/F7</f>
+        <v>1.5389279046440876E-3</v>
       </c>
       <c r="G13">
         <f t="shared" si="4"/>
-        <v>1.5740174050752208E-3</v>
+        <v>1.589729078370464E-3</v>
       </c>
     </row>
-    <row r="14" spans="4:7" x14ac:dyDescent="0.35">
-      <c r="D14" s="4"/>
-      <c r="E14">
+    <row r="14" spans="4:8" x14ac:dyDescent="0.35">
+      <c r="D14" s="6"/>
+      <c r="E14" s="1">
         <f>1/E8</f>
-        <v>1.3875957267601997E-3</v>
-      </c>
-      <c r="F14">
-        <f t="shared" ref="E14:G14" si="5">1/F8</f>
-        <v>1.3824489616087148E-3</v>
-      </c>
-      <c r="G14">
+        <v>1.3933747621735705E-3</v>
+      </c>
+      <c r="F14" s="1">
+        <f t="shared" ref="F14:G14" si="5">1/F8</f>
+        <v>1.4248221332907455E-3</v>
+      </c>
+      <c r="G14" s="1">
         <f t="shared" si="5"/>
-        <v>1.3877132066958994E-3</v>
+        <v>1.4940871501034657E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="4:8" x14ac:dyDescent="0.35">
+      <c r="D15" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E15">
+        <f>E12 * 10^3</f>
+        <v>2.011606972229766</v>
+      </c>
+      <c r="F15">
+        <f t="shared" ref="F15:G15" si="6">F12 * 10^3</f>
+        <v>2.0419539866088656</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="6"/>
+        <v>2.0476613240247743</v>
+      </c>
+    </row>
+    <row r="16" spans="4:8" x14ac:dyDescent="0.35">
+      <c r="D16" s="4"/>
+      <c r="E16">
+        <f t="shared" ref="E16:G16" si="7">E13 * 10^3</f>
+        <v>1.5134386007570009</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="7"/>
+        <v>1.5389279046440876</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="7"/>
+        <v>1.5897290783704641</v>
+      </c>
+    </row>
+    <row r="17" spans="4:7" x14ac:dyDescent="0.35">
+      <c r="D17" s="4"/>
+      <c r="E17">
+        <f t="shared" ref="E17:G17" si="8">E14 * 10^3</f>
+        <v>1.3933747621735706</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="8"/>
+        <v>1.4248221332907456</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="8"/>
+        <v>1.4940871501034658</v>
+      </c>
+    </row>
+    <row r="19" spans="4:7" x14ac:dyDescent="0.35">
+      <c r="E19" t="s">
+        <v>13</v>
+      </c>
+      <c r="F19" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="4:7" x14ac:dyDescent="0.35">
+      <c r="D20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="4:7" x14ac:dyDescent="0.35">
+      <c r="D21">
+        <v>2</v>
+      </c>
+      <c r="E21">
+        <f>19884*8.314</f>
+        <v>165315.576</v>
+      </c>
+    </row>
+    <row r="22" spans="4:7" x14ac:dyDescent="0.35">
+      <c r="D22">
+        <v>3</v>
+      </c>
+      <c r="E22">
+        <f>14578*8.314</f>
+        <v>121201.492</v>
       </c>
     </row>
   </sheetData>

</xml_diff>